<commit_message>
Added histograms into Excel-file
</commit_message>
<xml_diff>
--- a/ahp.xlsx
+++ b/ahp.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dnikiforov\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\workspace\ahp\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -138,7 +138,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -148,12 +148,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -416,12 +410,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -720,7 +714,7 @@
   <dimension ref="A1:K140"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -747,18 +741,18 @@
       <c r="A5" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="51" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
-      <c r="E5" s="51"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="51"/>
-      <c r="H5" s="51"/>
-      <c r="I5" s="51"/>
-      <c r="J5" s="51"/>
-      <c r="K5" s="51"/>
+      <c r="B5" s="48" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="48"/>
+      <c r="K5" s="48"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13056,7 +13050,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -13629,7 +13625,7 @@
         <f t="array" ref="A28:A37">Иерархия!A23:A32</f>
         <v>Ничего не менять</v>
       </c>
-      <c r="B28" s="48">
+      <c r="B28" s="49">
         <f t="array" ref="B28:B37">MMULT(B15:K24, B2:B11)</f>
         <v>0.31851014987437437</v>
       </c>
@@ -13638,7 +13634,7 @@
       <c r="A29" s="1" t="str">
         <v>Переехать в Москву</v>
       </c>
-      <c r="B29" s="49">
+      <c r="B29" s="50">
         <v>0.12266660468182783</v>
       </c>
     </row>
@@ -13646,7 +13642,7 @@
       <c r="A30" s="1" t="str">
         <v>Переехать за границу</v>
       </c>
-      <c r="B30" s="49">
+      <c r="B30" s="50">
         <v>0.20488655638064068</v>
       </c>
     </row>
@@ -13654,7 +13650,7 @@
       <c r="A31" s="1" t="str">
         <v>Фриланс</v>
       </c>
-      <c r="B31" s="49">
+      <c r="B31" s="50">
         <v>0.35393668906315712</v>
       </c>
     </row>
@@ -13662,7 +13658,7 @@
       <c r="A32" s="1" t="str">
         <v/>
       </c>
-      <c r="B32" s="49">
+      <c r="B32" s="50">
         <v>0</v>
       </c>
     </row>
@@ -13670,7 +13666,7 @@
       <c r="A33" s="1" t="str">
         <v/>
       </c>
-      <c r="B33" s="49">
+      <c r="B33" s="50">
         <v>0</v>
       </c>
     </row>
@@ -13678,7 +13674,7 @@
       <c r="A34" s="1" t="str">
         <v/>
       </c>
-      <c r="B34" s="49">
+      <c r="B34" s="50">
         <v>0</v>
       </c>
     </row>
@@ -13686,7 +13682,7 @@
       <c r="A35" s="1" t="str">
         <v/>
       </c>
-      <c r="B35" s="49">
+      <c r="B35" s="50">
         <v>0</v>
       </c>
     </row>
@@ -13694,7 +13690,7 @@
       <c r="A36" s="1" t="str">
         <v/>
       </c>
-      <c r="B36" s="49">
+      <c r="B36" s="50">
         <v>0</v>
       </c>
     </row>
@@ -13702,17 +13698,185 @@
       <c r="A37" s="2" t="str">
         <v/>
       </c>
-      <c r="B37" s="50">
+      <c r="B37" s="51">
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B15:B24">
+    <cfRule type="dataBar" priority="12">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{FD5E8E37-B366-496C-A37E-26C0778661FE}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C15:C24">
+    <cfRule type="dataBar" priority="11">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{9B822ED6-5044-4B99-8571-A424F9744AA0}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D15:D24">
+    <cfRule type="dataBar" priority="10">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{77F23AE3-6A76-4F05-BD77-33BC6E3840D0}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E15:E24">
+    <cfRule type="dataBar" priority="9">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{FA36375F-5DFF-4988-9BE9-2CA2B945B63C}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F15:F24">
+    <cfRule type="dataBar" priority="8">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{84143EBD-6212-4319-BE66-3A6713601501}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G15:G24">
+    <cfRule type="dataBar" priority="7">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{3152E7E4-E81A-48D4-8525-287163E61824}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H15:H24">
+    <cfRule type="dataBar" priority="6">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{EDBFEA8F-B845-42FF-A844-38F9475A9A01}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I15:I24">
+    <cfRule type="dataBar" priority="5">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{697F7F67-4D7E-44A7-A8E4-98D52D09911F}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J15:J24">
+    <cfRule type="dataBar" priority="4">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{63C8D6AB-493B-4B60-BB34-6CAD431A92E9}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K15:K24">
+    <cfRule type="dataBar" priority="3">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{96734944-53D9-408B-9F5F-3C0E010E1274}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B11">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{5C7A6639-BAA6-45BA-AD57-9EA58440DE18}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B28:B37">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{2C23254F-EB4F-43F4-BF8E-CD1B457BB5F9}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="2" id="{D7DD4F4A-1082-4841-B335-1B9DDA87FAE4}">
+          <x14:cfRule type="iconSet" priority="14" id="{D7DD4F4A-1082-4841-B335-1B9DDA87FAE4}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -13731,7 +13895,7 @@
           <xm:sqref>B25:K25</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="1" id="{2BAD0448-4D7E-40E4-BCAB-F8AE6C920193}">
+          <x14:cfRule type="iconSet" priority="13" id="{2BAD0448-4D7E-40E4-BCAB-F8AE6C920193}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -13749,6 +13913,162 @@
           </x14:cfRule>
           <xm:sqref>B12</xm:sqref>
         </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{FD5E8E37-B366-496C-A37E-26C0778661FE}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>B15:B24</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{9B822ED6-5044-4B99-8571-A424F9744AA0}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>C15:C24</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{77F23AE3-6A76-4F05-BD77-33BC6E3840D0}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D15:D24</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{FA36375F-5DFF-4988-9BE9-2CA2B945B63C}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E15:E24</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{84143EBD-6212-4319-BE66-3A6713601501}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F15:F24</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{3152E7E4-E81A-48D4-8525-287163E61824}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>G15:G24</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{EDBFEA8F-B845-42FF-A844-38F9475A9A01}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H15:H24</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{697F7F67-4D7E-44A7-A8E4-98D52D09911F}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>I15:I24</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{63C8D6AB-493B-4B60-BB34-6CAD431A92E9}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>J15:J24</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{96734944-53D9-408B-9F5F-3C0E010E1274}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>K15:K24</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{5C7A6639-BAA6-45BA-AD57-9EA58440DE18}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>B2:B11</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{2C23254F-EB4F-43F4-BF8E-CD1B457BB5F9}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF63C384"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>B28:B37</xm:sqref>
+        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>

</xml_diff>